<commit_message>
Incluyo la explicacion general en el Excel.  Mejoro los titulos de los ejemplos.
</commit_message>
<xml_diff>
--- a/Valoracion Por ISIN - Especificacion por ejemplos.xlsx
+++ b/Valoracion Por ISIN - Especificacion por ejemplos.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orct\Source\Repos\algoritmos.cs.garantias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar centeno\Source\Repos\algoritmos.cs.garantias\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7365" tabRatio="911"/>
   </bookViews>
   <sheets>
-    <sheet name="Colones" sheetId="5" r:id="rId1"/>
-    <sheet name="Dolares" sheetId="3" r:id="rId2"/>
-    <sheet name="UDES Anotados En Cuenta" sheetId="2" r:id="rId3"/>
-    <sheet name="UDES No anotados en cuenta" sheetId="6" r:id="rId4"/>
+    <sheet name="Explicación" sheetId="7" r:id="rId1"/>
+    <sheet name="Colones" sheetId="5" r:id="rId2"/>
+    <sheet name="Dolares" sheetId="3" r:id="rId3"/>
+    <sheet name="UDES Anotados En Cuenta" sheetId="2" r:id="rId4"/>
+    <sheet name="UDES No anotados en cuenta" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="35">
   <si>
     <t>ISIN</t>
   </si>
@@ -35,9 +36,6 @@
     <t>HDA000000000001</t>
   </si>
   <si>
-    <t>ISIN En UDES Anotados En Cuenta</t>
-  </si>
-  <si>
     <t>Ejemplo: cumple los días mínimos al vencimiento del emisor y se tiene el tipo de cambio de hoy</t>
   </si>
   <si>
@@ -83,23 +81,65 @@
     <t>Ejemplo: no cumple los días mínimos al vencimiento del emisor</t>
   </si>
   <si>
-    <t>ISIN En Colones</t>
-  </si>
-  <si>
     <t>Ejemplo: cumple los días mínimos al vencimiento del emisor</t>
   </si>
   <si>
-    <t>ISIN En Dolares</t>
-  </si>
-  <si>
-    <t>ISIN En UDES No Anotados En Cuenta</t>
+    <t>Valoración de un ISIN en UDES No Anotados En Cuenta</t>
+  </si>
+  <si>
+    <t>Valoración de un ISIN en Colones</t>
+  </si>
+  <si>
+    <t>Valoración de un ISIN en Dolares</t>
+  </si>
+  <si>
+    <t>Valoración de un ISIN en UDES Anotados En Cuenta</t>
+  </si>
+  <si>
+    <t>Valoración de emisiones por ISIN</t>
+  </si>
+  <si>
+    <t>Un ISIN es una emisión de valores que serán puestos en garantía por las operaciones de la entidad. Cuando se valora un ISIN se genera la siguiente información:</t>
+  </si>
+  <si>
+    <t>Campo</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>El número que identifica a la emisión</t>
+  </si>
+  <si>
+    <t>El porcentaje con que se valoró el aporte</t>
+  </si>
+  <si>
+    <t>El monto valorado para calcular el aporte</t>
+  </si>
+  <si>
+    <t>El monto con que se valora la emisión</t>
+  </si>
+  <si>
+    <t>Hay cuatro tipos de emisiones:</t>
+  </si>
+  <si>
+    <t>1. En colones</t>
+  </si>
+  <si>
+    <t>2. En dólares</t>
+  </si>
+  <si>
+    <t>3. En UDES anotados en cuenta</t>
+  </si>
+  <si>
+    <t>4. En UDES no anotados en cuenta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +179,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -185,10 +233,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -224,8 +273,16 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -538,22 +595,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45" customWidth="1"/>
+    <col min="3" max="6" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -561,7 +718,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -569,22 +726,22 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -612,7 +769,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -620,13 +777,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -645,12 +802,12 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -658,22 +815,22 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -701,7 +858,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -709,13 +866,13 @@
         <v>0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -737,12 +894,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,12 +911,12 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -767,22 +924,22 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -810,7 +967,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -818,13 +975,13 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -843,12 +1000,12 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -856,22 +1013,22 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -899,7 +1056,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -907,13 +1064,13 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -935,7 +1092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
@@ -950,7 +1107,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -973,7 +1130,7 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -996,7 +1153,7 @@
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1012,28 +1169,28 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1078,7 +1235,7 @@
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1094,13 +1251,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -1139,7 +1296,7 @@
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1162,7 +1319,7 @@
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1178,28 +1335,28 @@
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1244,7 +1401,7 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1260,13 +1417,13 @@
         <v>0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1305,7 +1462,7 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1328,7 +1485,7 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1344,28 +1501,28 @@
         <v>0</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1410,7 +1567,7 @@
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1426,13 +1583,13 @@
         <v>0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -1465,30 +1622,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" s="12"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1496,22 +1653,22 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1539,7 +1696,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1547,13 +1704,13 @@
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1572,12 +1729,12 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1585,22 +1742,22 @@
         <v>0</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1628,7 +1785,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1636,13 +1793,13 @@
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>